<commit_message>
File renames and associate batch file updates
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B48E3-921C-4B65-B9E8-80CC82EDE69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B325C8-69F9-4FFB-B206-29BAA2ECD405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="150" windowWidth="26265" windowHeight="18915" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15525" yWindow="300" windowWidth="21705" windowHeight="18345" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Parameter</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Vehicles File</t>
   </si>
   <si>
-    <t>Fuel Scenario Annual Data File</t>
-  </si>
-  <si>
     <t>Fuels File</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>context_fuel_prices.csv</t>
   </si>
   <si>
-    <t>context_fuel_upstream.csv</t>
-  </si>
-  <si>
     <t>context_new_vehicle_market.csv</t>
   </si>
   <si>
@@ -251,31 +245,34 @@
     <t>annual_vmt_fixed_by_age.csv</t>
   </si>
   <si>
-    <t>context_cost_factors-criteria.csv</t>
-  </si>
-  <si>
-    <t>context_cost_factors-scc.csv</t>
-  </si>
-  <si>
-    <t>context_cost_factors-energysecurity.csv</t>
-  </si>
-  <si>
-    <t>context_cost_factors-congestion-noise.csv</t>
-  </si>
-  <si>
-    <t>context_emission_factors-powersector.csv</t>
-  </si>
-  <si>
-    <t>context_emission_factors-refinery.csv</t>
-  </si>
-  <si>
-    <t>context_emission_factors-vehicles.csv</t>
-  </si>
-  <si>
-    <t>context_implicit_price_deflators.csv</t>
-  </si>
-  <si>
-    <t>context_cpi_price_deflators.csv</t>
+    <t>fuel_upstream.csv</t>
+  </si>
+  <si>
+    <t>cost_factors-criteria.csv</t>
+  </si>
+  <si>
+    <t>cost_factors-scc.csv</t>
+  </si>
+  <si>
+    <t>cost_factors-energysecurity.csv</t>
+  </si>
+  <si>
+    <t>cost_factors-congestion-noise.csv</t>
+  </si>
+  <si>
+    <t>emission_factors-powersector.csv</t>
+  </si>
+  <si>
+    <t>emission_factors-refinery.csv</t>
+  </si>
+  <si>
+    <t>emission_factors-vehicles.csv</t>
+  </si>
+  <si>
+    <t>implicit_price_deflators.csv</t>
+  </si>
+  <si>
+    <t>cpi_price_deflators.csv</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -471,9 +468,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -795,11 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG51"/>
+  <dimension ref="A1:AG50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -902,7 +896,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -925,24 +919,24 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1020,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1091,10 +1085,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1120,10 +1114,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1149,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1172,16 +1166,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1201,16 +1195,16 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1230,16 +1224,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1259,16 +1253,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>62</v>
+      <c r="C19" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1288,16 +1282,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1317,16 +1311,16 @@
     </row>
     <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1344,47 +1338,47 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
     </row>
     <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>21</v>
+      <c r="A23" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>66</v>
+      <c r="D23" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1402,7 +1396,7 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
@@ -1410,39 +1404,39 @@
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-    </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1468,10 +1462,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1489,77 +1483,65 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-    </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
+      <c r="C28" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -1576,27 +1558,32 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-    </row>
-    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+    <row r="30" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+    </row>
+    <row r="31" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1613,27 +1600,34 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="8">
+        <v>5</v>
+      </c>
+      <c r="D32" s="8">
+        <v>5</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
@@ -1672,10 +1666,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D34" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1693,76 +1687,76 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>52</v>
+    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="8">
-        <v>1</v>
-      </c>
-      <c r="D35" s="8">
-        <v>1</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+    </row>
+    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="10" t="b">
+      <c r="C37" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="D37" s="8">
-        <v>0.75</v>
+      <c r="D37" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1782,16 +1776,16 @@
     </row>
     <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="8" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C38" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="D38" s="8">
+        <v>-0.5</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1810,18 +1804,10 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="8">
-        <v>-0.5</v>
-      </c>
-      <c r="D39" s="8">
-        <v>-0.5</v>
-      </c>
+      <c r="A39" s="8"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -1838,31 +1824,32 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-    </row>
-    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+    <row r="40" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+    </row>
+    <row r="41" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -1879,39 +1866,46 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="27" t="s">
         <v>71</v>
       </c>
       <c r="E43" s="8"/>
@@ -1930,104 +1924,104 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="27"/>
+      <c r="S44" s="27"/>
+    </row>
+    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+    </row>
+    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-    </row>
-    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="28"/>
-      <c r="Q45" s="28"/>
-      <c r="R45" s="28"/>
-      <c r="S45" s="28"/>
-    </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="28" t="s">
+      <c r="B46" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D46" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="28"/>
-      <c r="S46" s="28"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
     </row>
     <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="27" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="22"/>
@@ -2047,16 +2041,16 @@
       <c r="S47" s="22"/>
     </row>
     <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="27" t="s">
         <v>76</v>
       </c>
       <c r="E48" s="22"/>
@@ -2076,16 +2070,16 @@
       <c r="S48" s="22"/>
     </row>
     <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="25" t="s">
+      <c r="B49" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="27" t="s">
         <v>77</v>
       </c>
       <c r="E49" s="22"/>
@@ -2105,16 +2099,16 @@
       <c r="S49" s="22"/>
     </row>
     <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="28" t="s">
+      <c r="B50" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D50" s="27" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="22"/>
@@ -2133,35 +2127,6 @@
       <c r="R50" s="22"/>
       <c r="S50" s="22"/>
     </row>
-    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
created postproc_batch.py batch process collates simulation results into batch summary file then calls postproc_batch
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B325C8-69F9-4FFB-B206-29BAA2ECD405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D26550-2CA8-4428-BFDA-873D75A910F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="300" windowWidth="21705" windowHeight="18345" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1545" windowWidth="19770" windowHeight="17145" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -793,7 +793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>

</xml_diff>

<commit_message>
batch file updates for consumer pricing multipliers
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D26550-2CA8-4428-BFDA-873D75A910F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACD0F76-6738-4196-B363-B5B7DACD328F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1545" windowWidth="19770" windowHeight="17145" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="6645" windowWidth="21780" windowHeight="12615" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>Parameter</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>cpi_price_deflators.csv</t>
+  </si>
+  <si>
+    <t>Consumer Pricing Multiplier Min</t>
+  </si>
+  <si>
+    <t>Consumer Pricing Multiplier Max</t>
   </si>
 </sst>
 </file>
@@ -789,11 +795,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG50"/>
+  <dimension ref="A1:AG52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="10" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,255 +1809,255 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-    </row>
-    <row r="40" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-    </row>
-    <row r="41" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+    <row r="39" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="27">
+        <v>0.95</v>
+      </c>
+      <c r="D39" s="27">
+        <v>0.95</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+    </row>
+    <row r="40" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="D40" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+    </row>
+    <row r="41" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+    </row>
+    <row r="43" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-    </row>
-    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+    </row>
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="27" t="s">
+      <c r="B44" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D44" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-    </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+    </row>
+    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="27" t="s">
+      <c r="B45" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="27" t="s">
+      <c r="D45" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-    </row>
-    <row r="44" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+    </row>
+    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="27" t="s">
+      <c r="B46" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="D46" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="27"/>
-    </row>
-    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="27"/>
+      <c r="S46" s="27"/>
+    </row>
+    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="27" t="s">
+      <c r="B47" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D47" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-    </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-    </row>
-    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="22"/>
-      <c r="S47" s="22"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+      <c r="N47" s="27"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
+      <c r="Q47" s="27"/>
+      <c r="R47" s="27"/>
+      <c r="S47" s="27"/>
     </row>
     <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -2070,17 +2076,17 @@
       <c r="S48" s="22"/>
     </row>
     <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="26" t="s">
+      <c r="A49" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -2099,17 +2105,17 @@
       <c r="S49" s="22"/>
     </row>
     <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="26" t="s">
+      <c r="A50" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -2127,6 +2133,64 @@
       <c r="R50" s="22"/>
       <c r="S50" s="22"/>
     </row>
+    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+    </row>
+    <row r="52" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="22"/>
+      <c r="S52" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
batch file updates for P0 compensation
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACD0F76-6738-4196-B363-B5B7DACD328F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B5B995-3A0B-400E-8588-A098FC837A3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="6645" windowWidth="21780" windowHeight="12615" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14445" yWindow="4455" windowWidth="18255" windowHeight="15570" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>Parameter</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>Consumer Pricing Multiplier Max</t>
+  </si>
+  <si>
+    <t>Context New Vehicle Prices File</t>
+  </si>
+  <si>
+    <t>GENERATE {X.Y} / String</t>
+  </si>
+  <si>
+    <t>GENERATE context_new_vehicle_prices.csv</t>
   </si>
 </sst>
 </file>
@@ -795,11 +804,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG52"/>
+  <dimension ref="A1:AG53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,28 +954,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>9</v>
-      </c>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -983,90 +983,88 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="b">
+      <c r="C10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="b">
+      <c r="D10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-    </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-    </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-    </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1083,47 +1081,40 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
+    <row r="13" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1143,16 +1134,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1172,16 +1163,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1201,16 +1192,16 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1230,16 +1221,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1259,16 +1250,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>69</v>
+      <c r="C19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1288,16 +1279,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>61</v>
+      <c r="C20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1317,16 +1308,16 @@
     </row>
     <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1344,47 +1335,47 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-    </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1402,47 +1393,47 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>67</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1462,16 +1453,16 @@
     </row>
     <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1489,65 +1480,77 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-    </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="8" t="b">
+      <c r="C28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="8" t="b">
+      <c r="D29" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -1564,32 +1567,27 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1606,38 +1604,31 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="8">
-        <v>5</v>
-      </c>
-      <c r="D32" s="8">
-        <v>5</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1666,16 +1657,16 @@
     </row>
     <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D34" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1693,76 +1684,76 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="10" t="b">
+      <c r="C36" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C37" s="8">
         <v>0.75</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <v>0.75</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="8" t="b">
-        <v>1</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1782,16 +1773,16 @@
     </row>
     <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="8">
-        <v>-0.5</v>
-      </c>
-      <c r="D38" s="8">
-        <v>-0.5</v>
+        <v>11</v>
+      </c>
+      <c r="C38" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1809,47 +1800,47 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="26" t="s">
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="27">
-        <v>0.95</v>
-      </c>
-      <c r="D39" s="27">
-        <v>0.95</v>
-      </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
+      <c r="C39" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="D39" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="27">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="D40" s="27">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
@@ -1867,53 +1858,60 @@
       <c r="R40" s="27"/>
       <c r="S40" s="27"/>
     </row>
-    <row r="41" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-    </row>
-    <row r="42" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-    </row>
-    <row r="43" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
+    <row r="41" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="D41" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="27"/>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+    </row>
+    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -1930,47 +1928,40 @@
       <c r="R43" s="14"/>
       <c r="S43" s="14"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
+    <row r="44" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
@@ -1988,47 +1979,47 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="26" t="s">
+    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="27"/>
+        <v>71</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="27"/>
@@ -2047,46 +2038,46 @@
       <c r="S47" s="27"/>
     </row>
     <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
+        <v>73</v>
+      </c>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="27"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
+      <c r="Q48" s="27"/>
+      <c r="R48" s="27"/>
+      <c r="S48" s="27"/>
     </row>
     <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -2106,16 +2097,16 @@
     </row>
     <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -2134,17 +2125,17 @@
       <c r="S50" s="22"/>
     </row>
     <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="26" t="s">
+      <c r="A51" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
@@ -2163,17 +2154,17 @@
       <c r="S51" s="22"/>
     </row>
     <row r="52" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
-        <v>48</v>
+      <c r="A52" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="B52" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -2191,6 +2182,35 @@
       <c r="R52" s="22"/>
       <c r="S52" s="22"/>
     </row>
+    <row r="53" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="22"/>
+      <c r="S53" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
working on fuel upstream calculation method selection
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
   <si>
     <t>Parameter</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>fuel_upstream.csv</t>
+  </si>
+  <si>
+    <t>Policy Fuel Upstream Methods File</t>
+  </si>
+  <si>
+    <t>fuel_upstream_methods.csv</t>
   </si>
   <si>
     <t>Context Fuel Prices File</t>
@@ -839,17 +845,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -877,10 +883,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1128,12 +1134,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1420,7 +1426,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1448,10 +1454,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1702,7 +1708,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG53"/>
+  <dimension ref="A1:AG54"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2628,7 +2634,7 @@
         <v>41</v>
       </c>
       <c r="D23" t="s" s="21">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -2662,13 +2668,13 @@
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" t="s" s="21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s" s="28">
         <v>5</v>
       </c>
       <c r="C24" t="s" s="21">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s" s="21">
         <v>44</v>
@@ -2836,14 +2842,14 @@
       <c r="A28" t="s" s="21">
         <v>51</v>
       </c>
-      <c r="B28" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C28" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D28" t="b" s="23">
-        <v>0</v>
+      <c r="B28" t="s" s="28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s" s="21">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s" s="21">
+        <v>52</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -2877,16 +2883,16 @@
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" t="s" s="21">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s" s="22">
         <v>17</v>
       </c>
       <c r="C29" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -2919,10 +2925,18 @@
       <c r="AG29" s="27"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="30"/>
+      <c r="A30" t="s" s="21">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C30" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b" s="23">
+        <v>1</v>
+      </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
@@ -2954,126 +2968,118 @@
       <c r="AG30" s="27"/>
     </row>
     <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="17"/>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="17"/>
-      <c r="AB31" s="17"/>
-      <c r="AC31" s="17"/>
-      <c r="AD31" s="17"/>
-      <c r="AE31" s="17"/>
-      <c r="AF31" s="17"/>
-      <c r="AG31" s="17"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" t="s" s="19">
-        <v>53</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
-      <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
-      <c r="AD32" s="20"/>
-      <c r="AE32" s="20"/>
-      <c r="AF32" s="20"/>
-      <c r="AG32" s="20"/>
-    </row>
-    <row r="33" ht="13.55" customHeight="1">
-      <c r="A33" t="s" s="21">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s" s="22">
+      <c r="A31" s="29"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="26"/>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="26"/>
+      <c r="AE31" s="26"/>
+      <c r="AF31" s="26"/>
+      <c r="AG31" s="27"/>
+    </row>
+    <row r="32" ht="13.55" customHeight="1">
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="17"/>
+      <c r="AG32" s="17"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1">
+      <c r="A33" t="s" s="19">
         <v>55</v>
       </c>
-      <c r="C33" s="23">
-        <v>5</v>
-      </c>
-      <c r="D33" s="23">
-        <v>5</v>
-      </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="25"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="26"/>
-      <c r="AB33" s="26"/>
-      <c r="AC33" s="26"/>
-      <c r="AD33" s="26"/>
-      <c r="AE33" s="26"/>
-      <c r="AF33" s="26"/>
-      <c r="AG33" s="27"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="20"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="20"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="20"/>
+      <c r="AE33" s="20"/>
+      <c r="AF33" s="20"/>
+      <c r="AG33" s="20"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" t="s" s="21">
         <v>56</v>
       </c>
       <c r="B34" t="s" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C34" s="23">
         <v>5</v>
@@ -3113,16 +3119,16 @@
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s" s="22">
         <v>57</v>
       </c>
-      <c r="B35" t="s" s="22">
-        <v>55</v>
-      </c>
       <c r="C35" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D35" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -3156,16 +3162,16 @@
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" t="s" s="21">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C36" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s" s="21">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="C36" s="23">
+        <v>1</v>
+      </c>
+      <c r="D36" s="23">
+        <v>1</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -3201,14 +3207,14 @@
       <c r="A37" t="s" s="21">
         <v>60</v>
       </c>
-      <c r="B37" t="s" s="28">
-        <v>55</v>
-      </c>
-      <c r="C37" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="D37" s="23">
-        <v>0.75</v>
+      <c r="B37" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C37" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s" s="21">
+        <v>61</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -3242,16 +3248,16 @@
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" t="s" s="21">
-        <v>61</v>
-      </c>
-      <c r="B38" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C38" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D38" t="b" s="23">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B38" t="s" s="28">
+        <v>57</v>
+      </c>
+      <c r="C38" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D38" s="23">
+        <v>0.75</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -3285,16 +3291,16 @@
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" t="s" s="21">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s" s="22">
-        <v>55</v>
-      </c>
-      <c r="C39" s="23">
-        <v>-0.5</v>
-      </c>
-      <c r="D39" s="23">
-        <v>-0.5</v>
+        <v>17</v>
+      </c>
+      <c r="C39" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D39" t="b" s="23">
+        <v>1</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -3328,16 +3334,16 @@
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" t="s" s="21">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C40" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="D40" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -3371,16 +3377,16 @@
     </row>
     <row r="41" ht="13.55" customHeight="1">
       <c r="A41" t="s" s="21">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C41" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="D41" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3413,10 +3419,18 @@
       <c r="AG41" s="27"/>
     </row>
     <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
+      <c r="A42" t="s" s="21">
+        <v>66</v>
+      </c>
+      <c r="B42" t="s" s="22">
+        <v>57</v>
+      </c>
+      <c r="C42" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D42" s="23">
+        <v>1.05</v>
+      </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
@@ -3448,119 +3462,111 @@
       <c r="AG42" s="27"/>
     </row>
     <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="17"/>
-      <c r="U43" s="17"/>
-      <c r="V43" s="17"/>
-      <c r="W43" s="17"/>
-      <c r="X43" s="17"/>
-      <c r="Y43" s="17"/>
-      <c r="Z43" s="17"/>
-      <c r="AA43" s="17"/>
-      <c r="AB43" s="17"/>
-      <c r="AC43" s="17"/>
-      <c r="AD43" s="17"/>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="17"/>
-    </row>
-    <row r="44" ht="18.75" customHeight="1">
-      <c r="A44" t="s" s="19">
-        <v>65</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
-      <c r="AA44" s="20"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="20"/>
-      <c r="AE44" s="20"/>
-      <c r="AF44" s="20"/>
-      <c r="AG44" s="20"/>
-    </row>
-    <row r="45" ht="13.55" customHeight="1">
-      <c r="A45" t="s" s="21">
-        <v>66</v>
-      </c>
-      <c r="B45" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C45" t="s" s="21">
+      <c r="A43" s="24"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="24"/>
+      <c r="T43" s="25"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="26"/>
+      <c r="AB43" s="26"/>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="26"/>
+      <c r="AE43" s="26"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="27"/>
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+      <c r="Y44" s="17"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="17"/>
+      <c r="AB44" s="17"/>
+      <c r="AC44" s="17"/>
+      <c r="AD44" s="17"/>
+      <c r="AE44" s="17"/>
+      <c r="AF44" s="17"/>
+      <c r="AG44" s="17"/>
+    </row>
+    <row r="45" ht="18.75" customHeight="1">
+      <c r="A45" t="s" s="19">
         <v>67</v>
       </c>
-      <c r="D45" t="s" s="21">
-        <v>67</v>
-      </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="25"/>
-      <c r="U45" s="26"/>
-      <c r="V45" s="26"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
-      <c r="Z45" s="26"/>
-      <c r="AA45" s="26"/>
-      <c r="AB45" s="26"/>
-      <c r="AC45" s="26"/>
-      <c r="AD45" s="26"/>
-      <c r="AE45" s="26"/>
-      <c r="AF45" s="26"/>
-      <c r="AG45" s="27"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="20"/>
+      <c r="AA45" s="20"/>
+      <c r="AB45" s="20"/>
+      <c r="AC45" s="20"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
       <c r="A46" t="s" s="21">
@@ -3906,6 +3912,49 @@
       <c r="AF53" s="26"/>
       <c r="AG53" s="27"/>
     </row>
+    <row r="54" ht="13.55" customHeight="1">
+      <c r="A54" t="s" s="21">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s" s="22">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s" s="21">
+        <v>85</v>
+      </c>
+      <c r="D54" t="s" s="21">
+        <v>85</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+      <c r="Q54" s="24"/>
+      <c r="R54" s="24"/>
+      <c r="S54" s="24"/>
+      <c r="T54" s="25"/>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="26"/>
+      <c r="X54" s="26"/>
+      <c r="Y54" s="26"/>
+      <c r="Z54" s="26"/>
+      <c r="AA54" s="26"/>
+      <c r="AB54" s="26"/>
+      <c r="AC54" s="26"/>
+      <c r="AD54" s="26"/>
+      <c r="AE54" s="26"/>
+      <c r="AF54" s="26"/>
+      <c r="AG54" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
adding drive cycle files to batch process
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>Parameter</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>fuel_upstream_methods.csv</t>
+  </si>
+  <si>
+    <t>Drive Cycles File</t>
+  </si>
+  <si>
+    <t>drive_cycles.csv</t>
+  </si>
+  <si>
+    <t>Drive Cycle Weights File</t>
+  </si>
+  <si>
+    <t>drive_cycle_weights.csv</t>
   </si>
   <si>
     <t>Context Fuel Prices File</t>
@@ -1708,7 +1720,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG54"/>
+  <dimension ref="A1:AG56"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2677,7 +2689,7 @@
         <v>43</v>
       </c>
       <c r="D24" t="s" s="21">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -2711,16 +2723,16 @@
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" t="s" s="21">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s" s="28">
         <v>5</v>
       </c>
       <c r="C25" t="s" s="21">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s" s="21">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
@@ -2754,13 +2766,13 @@
     </row>
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" t="s" s="21">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s" s="28">
         <v>5</v>
       </c>
       <c r="C26" t="s" s="21">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s" s="21">
         <v>48</v>
@@ -2885,14 +2897,14 @@
       <c r="A29" t="s" s="21">
         <v>53</v>
       </c>
-      <c r="B29" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C29" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D29" t="b" s="23">
-        <v>0</v>
+      <c r="B29" t="s" s="28">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s" s="21">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s" s="21">
+        <v>54</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -2926,16 +2938,16 @@
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" t="s" s="21">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C30" t="b" s="23">
-        <v>1</v>
-      </c>
-      <c r="D30" t="b" s="23">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="B30" t="s" s="28">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s" s="21">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s" s="21">
+        <v>56</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -2968,10 +2980,18 @@
       <c r="AG30" s="27"/>
     </row>
     <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="30"/>
+      <c r="A31" t="s" s="21">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C31" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D31" t="b" s="23">
+        <v>0</v>
+      </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
@@ -3003,175 +3023,167 @@
       <c r="AG31" s="27"/>
     </row>
     <row r="32" ht="13.55" customHeight="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
-      <c r="AC32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" t="s" s="19">
-        <v>55</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
-      <c r="Y33" s="20"/>
-      <c r="Z33" s="20"/>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
-      <c r="AD33" s="20"/>
-      <c r="AE33" s="20"/>
-      <c r="AF33" s="20"/>
-      <c r="AG33" s="20"/>
+      <c r="A32" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C32" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="26"/>
+      <c r="AG32" s="27"/>
+    </row>
+    <row r="33" ht="13.55" customHeight="1">
+      <c r="A33" s="29"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="26"/>
+      <c r="AE33" s="26"/>
+      <c r="AF33" s="26"/>
+      <c r="AG33" s="27"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" t="s" s="21">
-        <v>56</v>
-      </c>
-      <c r="B34" t="s" s="22">
-        <v>57</v>
-      </c>
-      <c r="C34" s="23">
-        <v>5</v>
-      </c>
-      <c r="D34" s="23">
-        <v>5</v>
-      </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="25"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="26"/>
-      <c r="AB34" s="26"/>
-      <c r="AC34" s="26"/>
-      <c r="AD34" s="26"/>
-      <c r="AE34" s="26"/>
-      <c r="AF34" s="26"/>
-      <c r="AG34" s="27"/>
-    </row>
-    <row r="35" ht="13.55" customHeight="1">
-      <c r="A35" t="s" s="21">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s" s="22">
-        <v>57</v>
-      </c>
-      <c r="C35" s="23">
-        <v>5</v>
-      </c>
-      <c r="D35" s="23">
-        <v>5</v>
-      </c>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AA35" s="26"/>
-      <c r="AB35" s="26"/>
-      <c r="AC35" s="26"/>
-      <c r="AD35" s="26"/>
-      <c r="AE35" s="26"/>
-      <c r="AF35" s="26"/>
-      <c r="AG35" s="27"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="17"/>
+    </row>
+    <row r="35" ht="18.75" customHeight="1">
+      <c r="A35" t="s" s="19">
+        <v>59</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="20"/>
+      <c r="AB35" s="20"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
+      <c r="AE35" s="20"/>
+      <c r="AF35" s="20"/>
+      <c r="AG35" s="20"/>
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" t="s" s="21">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s" s="22">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C36" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D36" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -3205,16 +3217,16 @@
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" t="s" s="21">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C37" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s" s="21">
         <v>61</v>
+      </c>
+      <c r="C37" s="23">
+        <v>5</v>
+      </c>
+      <c r="D37" s="23">
+        <v>5</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -3248,16 +3260,16 @@
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" t="s" s="21">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s" s="28">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="B38" t="s" s="22">
+        <v>61</v>
       </c>
       <c r="C38" s="23">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D38" s="23">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -3291,7 +3303,7 @@
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" t="s" s="21">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s" s="22">
         <v>17</v>
@@ -3299,8 +3311,8 @@
       <c r="C39" t="b" s="23">
         <v>0</v>
       </c>
-      <c r="D39" t="b" s="23">
-        <v>1</v>
+      <c r="D39" t="s" s="21">
+        <v>65</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -3334,16 +3346,16 @@
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" t="s" s="21">
-        <v>64</v>
-      </c>
-      <c r="B40" t="s" s="22">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="B40" t="s" s="28">
+        <v>61</v>
       </c>
       <c r="C40" s="23">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D40" s="23">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -3377,16 +3389,16 @@
     </row>
     <row r="41" ht="13.55" customHeight="1">
       <c r="A41" t="s" s="21">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s" s="22">
-        <v>57</v>
-      </c>
-      <c r="C41" s="23">
-        <v>0.95</v>
-      </c>
-      <c r="D41" s="23">
-        <v>0.95</v>
+        <v>17</v>
+      </c>
+      <c r="C41" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D41" t="b" s="23">
+        <v>1</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3420,16 +3432,16 @@
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" t="s" s="21">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s" s="22">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C42" s="23">
-        <v>1.05</v>
+        <v>-0.5</v>
       </c>
       <c r="D42" s="23">
-        <v>1.05</v>
+        <v>-0.5</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3462,10 +3474,18 @@
       <c r="AG42" s="27"/>
     </row>
     <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" s="24"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+      <c r="A43" t="s" s="21">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s" s="22">
+        <v>61</v>
+      </c>
+      <c r="C43" s="23">
+        <v>0.95</v>
+      </c>
+      <c r="D43" s="23">
+        <v>0.95</v>
+      </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
@@ -3497,162 +3517,154 @@
       <c r="AG43" s="27"/>
     </row>
     <row r="44" ht="13.55" customHeight="1">
-      <c r="A44" s="16"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="17"/>
-      <c r="U44" s="17"/>
-      <c r="V44" s="17"/>
-      <c r="W44" s="17"/>
-      <c r="X44" s="17"/>
-      <c r="Y44" s="17"/>
-      <c r="Z44" s="17"/>
-      <c r="AA44" s="17"/>
-      <c r="AB44" s="17"/>
-      <c r="AC44" s="17"/>
-      <c r="AD44" s="17"/>
-      <c r="AE44" s="17"/>
-      <c r="AF44" s="17"/>
-      <c r="AG44" s="17"/>
-    </row>
-    <row r="45" ht="18.75" customHeight="1">
-      <c r="A45" t="s" s="19">
-        <v>67</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="20"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
-      <c r="AA45" s="20"/>
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="20"/>
-      <c r="AE45" s="20"/>
-      <c r="AF45" s="20"/>
-      <c r="AG45" s="20"/>
+      <c r="A44" t="s" s="21">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s" s="22">
+        <v>61</v>
+      </c>
+      <c r="C44" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D44" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
+      <c r="Y44" s="26"/>
+      <c r="Z44" s="26"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
+      <c r="AD44" s="26"/>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="27"/>
+    </row>
+    <row r="45" ht="13.55" customHeight="1">
+      <c r="A45" s="24"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
+      <c r="Q45" s="24"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="25"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="26"/>
+      <c r="AA45" s="26"/>
+      <c r="AB45" s="26"/>
+      <c r="AC45" s="26"/>
+      <c r="AD45" s="26"/>
+      <c r="AE45" s="26"/>
+      <c r="AF45" s="26"/>
+      <c r="AG45" s="27"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" t="s" s="21">
-        <v>68</v>
-      </c>
-      <c r="B46" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s" s="21">
-        <v>69</v>
-      </c>
-      <c r="D46" t="s" s="21">
-        <v>69</v>
-      </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="25"/>
-      <c r="U46" s="26"/>
-      <c r="V46" s="26"/>
-      <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
-      <c r="Y46" s="26"/>
-      <c r="Z46" s="26"/>
-      <c r="AA46" s="26"/>
-      <c r="AB46" s="26"/>
-      <c r="AC46" s="26"/>
-      <c r="AD46" s="26"/>
-      <c r="AE46" s="26"/>
-      <c r="AF46" s="26"/>
-      <c r="AG46" s="27"/>
-    </row>
-    <row r="47" ht="13.55" customHeight="1">
-      <c r="A47" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="B47" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s" s="21">
+      <c r="A46" s="16"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="17"/>
+      <c r="AA46" s="17"/>
+      <c r="AB46" s="17"/>
+      <c r="AC46" s="17"/>
+      <c r="AD46" s="17"/>
+      <c r="AE46" s="17"/>
+      <c r="AF46" s="17"/>
+      <c r="AG46" s="17"/>
+    </row>
+    <row r="47" ht="18.75" customHeight="1">
+      <c r="A47" t="s" s="19">
         <v>71</v>
       </c>
-      <c r="D47" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="24"/>
-      <c r="S47" s="24"/>
-      <c r="T47" s="25"/>
-      <c r="U47" s="26"/>
-      <c r="V47" s="26"/>
-      <c r="W47" s="26"/>
-      <c r="X47" s="26"/>
-      <c r="Y47" s="26"/>
-      <c r="Z47" s="26"/>
-      <c r="AA47" s="26"/>
-      <c r="AB47" s="26"/>
-      <c r="AC47" s="26"/>
-      <c r="AD47" s="26"/>
-      <c r="AE47" s="26"/>
-      <c r="AF47" s="26"/>
-      <c r="AG47" s="27"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="20"/>
+      <c r="X47" s="20"/>
+      <c r="Y47" s="20"/>
+      <c r="Z47" s="20"/>
+      <c r="AA47" s="20"/>
+      <c r="AB47" s="20"/>
+      <c r="AC47" s="20"/>
+      <c r="AD47" s="20"/>
+      <c r="AE47" s="20"/>
+      <c r="AF47" s="20"/>
+      <c r="AG47" s="20"/>
     </row>
     <row r="48" ht="13.55" customHeight="1">
       <c r="A48" t="s" s="21">
@@ -3955,6 +3967,92 @@
       <c r="AF54" s="26"/>
       <c r="AG54" s="27"/>
     </row>
+    <row r="55" ht="13.55" customHeight="1">
+      <c r="A55" t="s" s="21">
+        <v>86</v>
+      </c>
+      <c r="B55" t="s" s="22">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s" s="21">
+        <v>87</v>
+      </c>
+      <c r="D55" t="s" s="21">
+        <v>87</v>
+      </c>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="24"/>
+      <c r="L55" s="24"/>
+      <c r="M55" s="24"/>
+      <c r="N55" s="24"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
+      <c r="Q55" s="24"/>
+      <c r="R55" s="24"/>
+      <c r="S55" s="24"/>
+      <c r="T55" s="25"/>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="26"/>
+      <c r="X55" s="26"/>
+      <c r="Y55" s="26"/>
+      <c r="Z55" s="26"/>
+      <c r="AA55" s="26"/>
+      <c r="AB55" s="26"/>
+      <c r="AC55" s="26"/>
+      <c r="AD55" s="26"/>
+      <c r="AE55" s="26"/>
+      <c r="AF55" s="26"/>
+      <c r="AG55" s="27"/>
+    </row>
+    <row r="56" ht="13.55" customHeight="1">
+      <c r="A56" t="s" s="21">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s" s="22">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s" s="21">
+        <v>89</v>
+      </c>
+      <c r="D56" t="s" s="21">
+        <v>89</v>
+      </c>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="24"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="24"/>
+      <c r="Q56" s="24"/>
+      <c r="R56" s="24"/>
+      <c r="S56" s="24"/>
+      <c r="T56" s="25"/>
+      <c r="U56" s="26"/>
+      <c r="V56" s="26"/>
+      <c r="W56" s="26"/>
+      <c r="X56" s="26"/>
+      <c r="Y56" s="26"/>
+      <c r="Z56" s="26"/>
+      <c r="AA56" s="26"/>
+      <c r="AB56" s="26"/>
+      <c r="AC56" s="26"/>
+      <c r="AD56" s="26"/>
+      <c r="AE56" s="26"/>
+      <c r="AF56" s="26"/>
+      <c r="AG56" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
working on required zev shares and production constraints
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>Parameter</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>required_zev_share.csv</t>
+  </si>
+  <si>
+    <t>Production Constraints File</t>
+  </si>
+  <si>
+    <t>production_constraints.csv</t>
   </si>
   <si>
     <t>Stock Deregistration File</t>
@@ -1720,7 +1726,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG56"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2983,14 +2989,14 @@
       <c r="A31" t="s" s="21">
         <v>57</v>
       </c>
-      <c r="B31" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C31" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D31" t="b" s="23">
-        <v>0</v>
+      <c r="B31" t="s" s="28">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s" s="21">
+        <v>58</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -3024,16 +3030,16 @@
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" t="s" s="21">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s" s="22">
         <v>17</v>
       </c>
       <c r="C32" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -3066,10 +3072,18 @@
       <c r="AG32" s="27"/>
     </row>
     <row r="33" ht="13.55" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="30"/>
+      <c r="A33" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C33" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="D33" t="b" s="23">
+        <v>1</v>
+      </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
@@ -3101,126 +3115,118 @@
       <c r="AG33" s="27"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17"/>
-      <c r="AG34" s="17"/>
-    </row>
-    <row r="35" ht="18.75" customHeight="1">
-      <c r="A35" t="s" s="19">
-        <v>59</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
-      <c r="Y35" s="20"/>
-      <c r="Z35" s="20"/>
-      <c r="AA35" s="20"/>
-      <c r="AB35" s="20"/>
-      <c r="AC35" s="20"/>
-      <c r="AD35" s="20"/>
-      <c r="AE35" s="20"/>
-      <c r="AF35" s="20"/>
-      <c r="AG35" s="20"/>
-    </row>
-    <row r="36" ht="13.55" customHeight="1">
-      <c r="A36" t="s" s="21">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s" s="22">
+      <c r="A34" s="29"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="26"/>
+      <c r="X34" s="26"/>
+      <c r="Y34" s="26"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="26"/>
+      <c r="AC34" s="26"/>
+      <c r="AD34" s="26"/>
+      <c r="AE34" s="26"/>
+      <c r="AF34" s="26"/>
+      <c r="AG34" s="27"/>
+    </row>
+    <row r="35" ht="13.55" customHeight="1">
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
+      <c r="AD35" s="17"/>
+      <c r="AE35" s="17"/>
+      <c r="AF35" s="17"/>
+      <c r="AG35" s="17"/>
+    </row>
+    <row r="36" ht="18.75" customHeight="1">
+      <c r="A36" t="s" s="19">
         <v>61</v>
       </c>
-      <c r="C36" s="23">
-        <v>5</v>
-      </c>
-      <c r="D36" s="23">
-        <v>5</v>
-      </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="26"/>
-      <c r="V36" s="26"/>
-      <c r="W36" s="26"/>
-      <c r="X36" s="26"/>
-      <c r="Y36" s="26"/>
-      <c r="Z36" s="26"/>
-      <c r="AA36" s="26"/>
-      <c r="AB36" s="26"/>
-      <c r="AC36" s="26"/>
-      <c r="AD36" s="26"/>
-      <c r="AE36" s="26"/>
-      <c r="AF36" s="26"/>
-      <c r="AG36" s="27"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="20"/>
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" t="s" s="21">
         <v>62</v>
       </c>
       <c r="B37" t="s" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C37" s="23">
         <v>5</v>
@@ -3260,16 +3266,16 @@
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" t="s" s="21">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s" s="22">
         <v>63</v>
       </c>
-      <c r="B38" t="s" s="22">
-        <v>61</v>
-      </c>
       <c r="C38" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D38" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -3303,16 +3309,16 @@
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" t="s" s="21">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C39" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s" s="21">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="C39" s="23">
+        <v>1</v>
+      </c>
+      <c r="D39" s="23">
+        <v>1</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -3348,14 +3354,14 @@
       <c r="A40" t="s" s="21">
         <v>66</v>
       </c>
-      <c r="B40" t="s" s="28">
-        <v>61</v>
-      </c>
-      <c r="C40" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="D40" s="23">
-        <v>0.75</v>
+      <c r="B40" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C40" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s" s="21">
+        <v>67</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -3389,16 +3395,16 @@
     </row>
     <row r="41" ht="13.55" customHeight="1">
       <c r="A41" t="s" s="21">
-        <v>67</v>
-      </c>
-      <c r="B41" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C41" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D41" t="b" s="23">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B41" t="s" s="28">
+        <v>63</v>
+      </c>
+      <c r="C41" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D41" s="23">
+        <v>0.75</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3432,16 +3438,16 @@
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" t="s" s="21">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s" s="22">
-        <v>61</v>
-      </c>
-      <c r="C42" s="23">
-        <v>-0.5</v>
-      </c>
-      <c r="D42" s="23">
-        <v>-0.5</v>
+        <v>17</v>
+      </c>
+      <c r="C42" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D42" t="b" s="23">
+        <v>1</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3475,16 +3481,16 @@
     </row>
     <row r="43" ht="13.55" customHeight="1">
       <c r="A43" t="s" s="21">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C43" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="D43" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -3518,16 +3524,16 @@
     </row>
     <row r="44" ht="13.55" customHeight="1">
       <c r="A44" t="s" s="21">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C44" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="D44" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -3560,10 +3566,18 @@
       <c r="AG44" s="27"/>
     </row>
     <row r="45" ht="13.55" customHeight="1">
-      <c r="A45" s="24"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
+      <c r="A45" t="s" s="21">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s" s="22">
+        <v>63</v>
+      </c>
+      <c r="C45" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D45" s="23">
+        <v>1.05</v>
+      </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
@@ -3595,119 +3609,111 @@
       <c r="AG45" s="27"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="17"/>
-      <c r="U46" s="17"/>
-      <c r="V46" s="17"/>
-      <c r="W46" s="17"/>
-      <c r="X46" s="17"/>
-      <c r="Y46" s="17"/>
-      <c r="Z46" s="17"/>
-      <c r="AA46" s="17"/>
-      <c r="AB46" s="17"/>
-      <c r="AC46" s="17"/>
-      <c r="AD46" s="17"/>
-      <c r="AE46" s="17"/>
-      <c r="AF46" s="17"/>
-      <c r="AG46" s="17"/>
-    </row>
-    <row r="47" ht="18.75" customHeight="1">
-      <c r="A47" t="s" s="19">
-        <v>71</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="20"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
-      <c r="Y47" s="20"/>
-      <c r="Z47" s="20"/>
-      <c r="AA47" s="20"/>
-      <c r="AB47" s="20"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="20"/>
-      <c r="AE47" s="20"/>
-      <c r="AF47" s="20"/>
-      <c r="AG47" s="20"/>
-    </row>
-    <row r="48" ht="13.55" customHeight="1">
-      <c r="A48" t="s" s="21">
-        <v>72</v>
-      </c>
-      <c r="B48" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C48" t="s" s="21">
+      <c r="A46" s="24"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="25"/>
+      <c r="U46" s="26"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="26"/>
+      <c r="Z46" s="26"/>
+      <c r="AA46" s="26"/>
+      <c r="AB46" s="26"/>
+      <c r="AC46" s="26"/>
+      <c r="AD46" s="26"/>
+      <c r="AE46" s="26"/>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="27"/>
+    </row>
+    <row r="47" ht="13.55" customHeight="1">
+      <c r="A47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+      <c r="X47" s="17"/>
+      <c r="Y47" s="17"/>
+      <c r="Z47" s="17"/>
+      <c r="AA47" s="17"/>
+      <c r="AB47" s="17"/>
+      <c r="AC47" s="17"/>
+      <c r="AD47" s="17"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="17"/>
+      <c r="AG47" s="17"/>
+    </row>
+    <row r="48" ht="18.75" customHeight="1">
+      <c r="A48" t="s" s="19">
         <v>73</v>
       </c>
-      <c r="D48" t="s" s="21">
-        <v>73</v>
-      </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-      <c r="T48" s="25"/>
-      <c r="U48" s="26"/>
-      <c r="V48" s="26"/>
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
-      <c r="Y48" s="26"/>
-      <c r="Z48" s="26"/>
-      <c r="AA48" s="26"/>
-      <c r="AB48" s="26"/>
-      <c r="AC48" s="26"/>
-      <c r="AD48" s="26"/>
-      <c r="AE48" s="26"/>
-      <c r="AF48" s="26"/>
-      <c r="AG48" s="27"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+      <c r="Z48" s="20"/>
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="20"/>
+      <c r="AC48" s="20"/>
+      <c r="AD48" s="20"/>
+      <c r="AE48" s="20"/>
+      <c r="AF48" s="20"/>
+      <c r="AG48" s="20"/>
     </row>
     <row r="49" ht="13.55" customHeight="1">
       <c r="A49" t="s" s="21">
@@ -4053,6 +4059,49 @@
       <c r="AF56" s="26"/>
       <c r="AG56" s="27"/>
     </row>
+    <row r="57" ht="13.55" customHeight="1">
+      <c r="A57" t="s" s="21">
+        <v>90</v>
+      </c>
+      <c r="B57" t="s" s="22">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s" s="21">
+        <v>91</v>
+      </c>
+      <c r="D57" t="s" s="21">
+        <v>91</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="24"/>
+      <c r="L57" s="24"/>
+      <c r="M57" s="24"/>
+      <c r="N57" s="24"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="24"/>
+      <c r="Q57" s="24"/>
+      <c r="R57" s="24"/>
+      <c r="S57" s="24"/>
+      <c r="T57" s="25"/>
+      <c r="U57" s="26"/>
+      <c r="V57" s="26"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+      <c r="Y57" s="26"/>
+      <c r="Z57" s="26"/>
+      <c r="AA57" s="26"/>
+      <c r="AB57" s="26"/>
+      <c r="AC57" s="26"/>
+      <c r="AD57" s="26"/>
+      <c r="AE57" s="26"/>
+      <c r="AF57" s="26"/>
+      <c r="AG57" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
adding price modification inputs refactored the "policy" out of the name... modified the batch files / process for the new input file
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>Parameter</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>required_zev_share.csv</t>
+  </si>
+  <si>
+    <t>Price Modifications File</t>
+  </si>
+  <si>
+    <t>price_modifications.csv</t>
   </si>
   <si>
     <t>Production Constraints File</t>
@@ -1726,7 +1732,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:AG58"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3032,14 +3038,14 @@
       <c r="A32" t="s" s="21">
         <v>59</v>
       </c>
-      <c r="B32" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C32" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D32" t="b" s="23">
-        <v>0</v>
+      <c r="B32" t="s" s="28">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s" s="21">
+        <v>60</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -3073,16 +3079,16 @@
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" t="s" s="21">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s" s="22">
         <v>17</v>
       </c>
       <c r="C33" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -3115,10 +3121,18 @@
       <c r="AG33" s="27"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="30"/>
+      <c r="A34" t="s" s="21">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C34" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b" s="23">
+        <v>1</v>
+      </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
       <c r="G34" s="24"/>
@@ -3150,126 +3164,118 @@
       <c r="AG34" s="27"/>
     </row>
     <row r="35" ht="13.55" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="17"/>
-    </row>
-    <row r="36" ht="18.75" customHeight="1">
-      <c r="A36" t="s" s="19">
-        <v>61</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
-      <c r="Y36" s="20"/>
-      <c r="Z36" s="20"/>
-      <c r="AA36" s="20"/>
-      <c r="AB36" s="20"/>
-      <c r="AC36" s="20"/>
-      <c r="AD36" s="20"/>
-      <c r="AE36" s="20"/>
-      <c r="AF36" s="20"/>
-      <c r="AG36" s="20"/>
-    </row>
-    <row r="37" ht="13.55" customHeight="1">
-      <c r="A37" t="s" s="21">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s" s="22">
+      <c r="A35" s="29"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="26"/>
+      <c r="X35" s="26"/>
+      <c r="Y35" s="26"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+      <c r="AB35" s="26"/>
+      <c r="AC35" s="26"/>
+      <c r="AD35" s="26"/>
+      <c r="AE35" s="26"/>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="27"/>
+    </row>
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
+      <c r="AD36" s="17"/>
+      <c r="AE36" s="17"/>
+      <c r="AF36" s="17"/>
+      <c r="AG36" s="17"/>
+    </row>
+    <row r="37" ht="18.75" customHeight="1">
+      <c r="A37" t="s" s="19">
         <v>63</v>
       </c>
-      <c r="C37" s="23">
-        <v>5</v>
-      </c>
-      <c r="D37" s="23">
-        <v>5</v>
-      </c>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="26"/>
-      <c r="V37" s="26"/>
-      <c r="W37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-      <c r="AA37" s="26"/>
-      <c r="AB37" s="26"/>
-      <c r="AC37" s="26"/>
-      <c r="AD37" s="26"/>
-      <c r="AE37" s="26"/>
-      <c r="AF37" s="26"/>
-      <c r="AG37" s="27"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="20"/>
+      <c r="AA37" s="20"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="20"/>
+      <c r="AG37" s="20"/>
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" t="s" s="21">
         <v>64</v>
       </c>
       <c r="B38" t="s" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C38" s="23">
         <v>5</v>
@@ -3309,16 +3315,16 @@
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" t="s" s="21">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s" s="22">
         <v>65</v>
       </c>
-      <c r="B39" t="s" s="22">
-        <v>63</v>
-      </c>
       <c r="C39" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D39" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -3352,16 +3358,16 @@
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" t="s" s="21">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C40" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s" s="21">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="C40" s="23">
+        <v>1</v>
+      </c>
+      <c r="D40" s="23">
+        <v>1</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -3397,14 +3403,14 @@
       <c r="A41" t="s" s="21">
         <v>68</v>
       </c>
-      <c r="B41" t="s" s="28">
-        <v>63</v>
-      </c>
-      <c r="C41" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="D41" s="23">
-        <v>0.75</v>
+      <c r="B41" t="s" s="22">
+        <v>17</v>
+      </c>
+      <c r="C41" t="b" s="23">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s" s="21">
+        <v>69</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3438,16 +3444,16 @@
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" t="s" s="21">
-        <v>69</v>
-      </c>
-      <c r="B42" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C42" t="b" s="23">
-        <v>1</v>
-      </c>
-      <c r="D42" t="b" s="23">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B42" t="s" s="28">
+        <v>65</v>
+      </c>
+      <c r="C42" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="23">
+        <v>0.75</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3481,16 +3487,16 @@
     </row>
     <row r="43" ht="13.55" customHeight="1">
       <c r="A43" t="s" s="21">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s" s="22">
-        <v>63</v>
-      </c>
-      <c r="C43" s="23">
-        <v>-0.5</v>
-      </c>
-      <c r="D43" s="23">
-        <v>-0.5</v>
+        <v>17</v>
+      </c>
+      <c r="C43" t="b" s="23">
+        <v>1</v>
+      </c>
+      <c r="D43" t="b" s="23">
+        <v>1</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -3524,16 +3530,16 @@
     </row>
     <row r="44" ht="13.55" customHeight="1">
       <c r="A44" t="s" s="21">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C44" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="D44" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -3567,16 +3573,16 @@
     </row>
     <row r="45" ht="13.55" customHeight="1">
       <c r="A45" t="s" s="21">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C45" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="D45" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -3609,10 +3615,18 @@
       <c r="AG45" s="27"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" s="24"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
+      <c r="A46" t="s" s="21">
+        <v>74</v>
+      </c>
+      <c r="B46" t="s" s="22">
+        <v>65</v>
+      </c>
+      <c r="C46" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D46" s="23">
+        <v>1.05</v>
+      </c>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
@@ -3644,119 +3658,111 @@
       <c r="AG46" s="27"/>
     </row>
     <row r="47" ht="13.55" customHeight="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="17"/>
-      <c r="U47" s="17"/>
-      <c r="V47" s="17"/>
-      <c r="W47" s="17"/>
-      <c r="X47" s="17"/>
-      <c r="Y47" s="17"/>
-      <c r="Z47" s="17"/>
-      <c r="AA47" s="17"/>
-      <c r="AB47" s="17"/>
-      <c r="AC47" s="17"/>
-      <c r="AD47" s="17"/>
-      <c r="AE47" s="17"/>
-      <c r="AF47" s="17"/>
-      <c r="AG47" s="17"/>
-    </row>
-    <row r="48" ht="18.75" customHeight="1">
-      <c r="A48" t="s" s="19">
-        <v>73</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="20"/>
-      <c r="U48" s="20"/>
-      <c r="V48" s="20"/>
-      <c r="W48" s="20"/>
-      <c r="X48" s="20"/>
-      <c r="Y48" s="20"/>
-      <c r="Z48" s="20"/>
-      <c r="AA48" s="20"/>
-      <c r="AB48" s="20"/>
-      <c r="AC48" s="20"/>
-      <c r="AD48" s="20"/>
-      <c r="AE48" s="20"/>
-      <c r="AF48" s="20"/>
-      <c r="AG48" s="20"/>
-    </row>
-    <row r="49" ht="13.55" customHeight="1">
-      <c r="A49" t="s" s="21">
-        <v>74</v>
-      </c>
-      <c r="B49" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C49" t="s" s="21">
+      <c r="A47" s="24"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="24"/>
+      <c r="R47" s="24"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="25"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
+      <c r="X47" s="26"/>
+      <c r="Y47" s="26"/>
+      <c r="Z47" s="26"/>
+      <c r="AA47" s="26"/>
+      <c r="AB47" s="26"/>
+      <c r="AC47" s="26"/>
+      <c r="AD47" s="26"/>
+      <c r="AE47" s="26"/>
+      <c r="AF47" s="26"/>
+      <c r="AG47" s="27"/>
+    </row>
+    <row r="48" ht="13.55" customHeight="1">
+      <c r="A48" s="16"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+      <c r="X48" s="17"/>
+      <c r="Y48" s="17"/>
+      <c r="Z48" s="17"/>
+      <c r="AA48" s="17"/>
+      <c r="AB48" s="17"/>
+      <c r="AC48" s="17"/>
+      <c r="AD48" s="17"/>
+      <c r="AE48" s="17"/>
+      <c r="AF48" s="17"/>
+      <c r="AG48" s="17"/>
+    </row>
+    <row r="49" ht="18.75" customHeight="1">
+      <c r="A49" t="s" s="19">
         <v>75</v>
       </c>
-      <c r="D49" t="s" s="21">
-        <v>75</v>
-      </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="24"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="24"/>
-      <c r="S49" s="24"/>
-      <c r="T49" s="25"/>
-      <c r="U49" s="26"/>
-      <c r="V49" s="26"/>
-      <c r="W49" s="26"/>
-      <c r="X49" s="26"/>
-      <c r="Y49" s="26"/>
-      <c r="Z49" s="26"/>
-      <c r="AA49" s="26"/>
-      <c r="AB49" s="26"/>
-      <c r="AC49" s="26"/>
-      <c r="AD49" s="26"/>
-      <c r="AE49" s="26"/>
-      <c r="AF49" s="26"/>
-      <c r="AG49" s="27"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+      <c r="Z49" s="20"/>
+      <c r="AA49" s="20"/>
+      <c r="AB49" s="20"/>
+      <c r="AC49" s="20"/>
+      <c r="AD49" s="20"/>
+      <c r="AE49" s="20"/>
+      <c r="AF49" s="20"/>
+      <c r="AG49" s="20"/>
     </row>
     <row r="50" ht="13.55" customHeight="1">
       <c r="A50" t="s" s="21">
@@ -4102,6 +4108,49 @@
       <c r="AF57" s="26"/>
       <c r="AG57" s="27"/>
     </row>
+    <row r="58" ht="13.55" customHeight="1">
+      <c r="A58" t="s" s="21">
+        <v>92</v>
+      </c>
+      <c r="B58" t="s" s="22">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s" s="21">
+        <v>93</v>
+      </c>
+      <c r="D58" t="s" s="21">
+        <v>93</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="24"/>
+      <c r="T58" s="25"/>
+      <c r="U58" s="26"/>
+      <c r="V58" s="26"/>
+      <c r="W58" s="26"/>
+      <c r="X58" s="26"/>
+      <c r="Y58" s="26"/>
+      <c r="Z58" s="26"/>
+      <c r="AA58" s="26"/>
+      <c r="AB58" s="26"/>
+      <c r="AC58" s="26"/>
+      <c r="AD58" s="26"/>
+      <c r="AE58" s="26"/>
+      <c r="AF58" s="26"/>
+      <c r="AG58" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
multiple_session_batch.xlsx, correction to add 'GHG Credits File' row.
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBolon\PycharmProjects\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23A305A-EDC7-4BA8-8C29-1B5E7901C31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1305" yWindow="1095" windowWidth="17895" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sessions" sheetId="1" r:id="rId4"/>
+    <sheet name="Sessions" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
   <si>
     <t>Parameter</t>
   </si>
@@ -293,42 +302,37 @@
   </si>
   <si>
     <t>cpi_price_deflators.csv</t>
+  </si>
+  <si>
+    <t>GHG Credits File</t>
+  </si>
+  <si>
+    <t>ghg_credits.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="16"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -547,105 +551,99 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,28 +654,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffc5deb5"/>
-      <rgbColor rgb="ffe2eeda"/>
-      <rgbColor rgb="ffd8d8d8"/>
-      <rgbColor rgb="fff2f2f2"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFC5DEB5"/>
+      <rgbColor rgb="FFE2EEDA"/>
+      <rgbColor rgb="FFD8D8D8"/>
+      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -879,7 +934,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -898,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -928,7 +983,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,7 +1009,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1035,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1006,7 +1061,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1032,7 +1087,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,7 +1113,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1084,7 +1139,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1110,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1136,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,9 +1204,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1168,7 +1229,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1187,7 +1248,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1274,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1300,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1352,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1378,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1404,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1430,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1395,7 +1456,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1482,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1434,9 +1495,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1450,7 +1517,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1469,7 +1536,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1499,7 +1566,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1525,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1551,7 +1618,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1577,7 +1644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1603,7 +1670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1629,7 +1696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1655,7 +1722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1681,7 +1748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1707,7 +1774,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1720,43 +1787,52 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="1" customWidth="1"/>
-    <col min="5" max="17" width="21.3516" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6719" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5" style="1" customWidth="1"/>
-    <col min="21" max="33" width="8.67188" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.67188" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
+    <col min="21" max="34" width="8.7109375" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5"/>
@@ -1790,8 +1866,8 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="7"/>
@@ -1827,14 +1903,14 @@
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="11">
+    <row r="3" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="12">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="13"/>
@@ -1868,11 +1944,11 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="14"/>
@@ -1907,14 +1983,14 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="12">
+    <row r="5" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="12">
+      <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s" s="12">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="15"/>
@@ -1948,14 +2024,14 @@
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="12">
+    <row r="6" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="12">
+      <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s" s="12">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="15"/>
@@ -1989,14 +2065,14 @@
       <c r="AF6" s="10"/>
       <c r="AG6" s="10"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="12">
+    <row r="7" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="12">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s" s="12">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="15"/>
@@ -2030,7 +2106,7 @@
       <c r="AF7" s="10"/>
       <c r="AG7" s="10"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -2065,8 +2141,8 @@
       <c r="AF8" s="10"/>
       <c r="AG8" s="10"/>
     </row>
-    <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" t="s" s="19">
+    <row r="9" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="7"/>
@@ -2102,17 +2178,17 @@
       <c r="AF9" s="20"/>
       <c r="AG9" s="20"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="21">
+    <row r="10" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s" s="22">
+      <c r="B10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="b" s="23">
+      <c r="C10" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="D10" t="b" s="23">
+      <c r="D10" s="23" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="24"/>
@@ -2145,17 +2221,17 @@
       <c r="AF10" s="26"/>
       <c r="AG10" s="27"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="21">
+    <row r="11" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s" s="28">
+      <c r="B11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s" s="21">
+      <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s" s="21">
+      <c r="D11" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="24"/>
@@ -2188,7 +2264,7 @@
       <c r="AF11" s="26"/>
       <c r="AG11" s="27"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -2223,8 +2299,8 @@
       <c r="AF12" s="17"/>
       <c r="AG12" s="17"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" t="s" s="19">
+    <row r="13" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="7"/>
@@ -2260,17 +2336,17 @@
       <c r="AF13" s="20"/>
       <c r="AG13" s="20"/>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="21">
+    <row r="14" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s" s="28">
+      <c r="B14" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s" s="21">
+      <c r="C14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s" s="21">
+      <c r="D14" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="24"/>
@@ -2303,17 +2379,17 @@
       <c r="AF14" s="26"/>
       <c r="AG14" s="27"/>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="21">
+    <row r="15" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s" s="28">
+      <c r="B15" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s" s="21">
+      <c r="C15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s" s="21">
+      <c r="D15" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="24"/>
@@ -2346,17 +2422,17 @@
       <c r="AF15" s="26"/>
       <c r="AG15" s="27"/>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="21">
+    <row r="16" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s" s="28">
+      <c r="B16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s" s="21">
+      <c r="C16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s" s="21">
+      <c r="D16" s="21" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="24"/>
@@ -2389,17 +2465,17 @@
       <c r="AF16" s="26"/>
       <c r="AG16" s="27"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" t="s" s="21">
+    <row r="17" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s" s="28">
+      <c r="B17" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="s" s="21">
+      <c r="C17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s" s="21">
+      <c r="D17" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="24"/>
@@ -2432,17 +2508,17 @@
       <c r="AF17" s="26"/>
       <c r="AG17" s="27"/>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="21">
+    <row r="18" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s" s="28">
+      <c r="B18" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="s" s="21">
+      <c r="C18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D18" t="s" s="21">
+      <c r="D18" s="21" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="24"/>
@@ -2475,17 +2551,17 @@
       <c r="AF18" s="26"/>
       <c r="AG18" s="27"/>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" t="s" s="21">
+    <row r="19" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s" s="28">
+      <c r="B19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C19" t="s" s="21">
+      <c r="C19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s" s="21">
+      <c r="D19" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="24"/>
@@ -2518,17 +2594,17 @@
       <c r="AF19" s="26"/>
       <c r="AG19" s="27"/>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" t="s" s="21">
+    <row r="20" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s" s="28">
+      <c r="B20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C20" t="s" s="21">
+      <c r="C20" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s" s="21">
+      <c r="D20" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="24"/>
@@ -2561,17 +2637,17 @@
       <c r="AF20" s="26"/>
       <c r="AG20" s="27"/>
     </row>
-    <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" t="s" s="21">
+    <row r="21" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s" s="28">
+      <c r="B21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C21" t="s" s="21">
+      <c r="C21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s" s="21">
+      <c r="D21" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="24"/>
@@ -2604,17 +2680,17 @@
       <c r="AF21" s="26"/>
       <c r="AG21" s="27"/>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" t="s" s="21">
+    <row r="22" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s" s="28">
+      <c r="B22" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s" s="21">
+      <c r="C22" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s" s="21">
+      <c r="D22" s="21" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="24"/>
@@ -2647,17 +2723,17 @@
       <c r="AF22" s="26"/>
       <c r="AG22" s="27"/>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" t="s" s="21">
+    <row r="23" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s" s="28">
+      <c r="B23" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C23" t="s" s="21">
+      <c r="C23" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s" s="21">
+      <c r="D23" s="21" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="24"/>
@@ -2690,17 +2766,17 @@
       <c r="AF23" s="26"/>
       <c r="AG23" s="27"/>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" t="s" s="21">
+    <row r="24" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s" s="28">
+      <c r="B24" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C24" t="s" s="21">
+      <c r="C24" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D24" t="s" s="21">
+      <c r="D24" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="24"/>
@@ -2733,17 +2809,17 @@
       <c r="AF24" s="26"/>
       <c r="AG24" s="27"/>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" t="s" s="21">
+    <row r="25" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s" s="28">
+      <c r="B25" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s" s="21">
+      <c r="C25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D25" t="s" s="21">
+      <c r="D25" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="24"/>
@@ -2776,17 +2852,17 @@
       <c r="AF25" s="26"/>
       <c r="AG25" s="27"/>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" t="s" s="21">
+    <row r="26" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s" s="28">
+      <c r="B26" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s" s="21">
+      <c r="C26" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D26" t="s" s="21">
+      <c r="D26" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="24"/>
@@ -2819,17 +2895,17 @@
       <c r="AF26" s="26"/>
       <c r="AG26" s="27"/>
     </row>
-    <row r="27" ht="13.55" customHeight="1">
-      <c r="A27" t="s" s="21">
+    <row r="27" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s" s="28">
+      <c r="B27" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s" s="21">
+      <c r="C27" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s" s="21">
+      <c r="D27" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="24"/>
@@ -2862,18 +2938,18 @@
       <c r="AF27" s="26"/>
       <c r="AG27" s="27"/>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" t="s" s="21">
-        <v>51</v>
-      </c>
-      <c r="B28" t="s" s="28">
+    <row r="28" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="s" s="21">
-        <v>52</v>
-      </c>
-      <c r="D28" t="s" s="21">
-        <v>52</v>
+      <c r="C28" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -2905,18 +2981,18 @@
       <c r="AF28" s="26"/>
       <c r="AG28" s="27"/>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" t="s" s="21">
-        <v>53</v>
-      </c>
-      <c r="B29" t="s" s="28">
+    <row r="29" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C29" t="s" s="21">
-        <v>54</v>
-      </c>
-      <c r="D29" t="s" s="21">
-        <v>54</v>
+      <c r="C29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -2948,18 +3024,18 @@
       <c r="AF29" s="26"/>
       <c r="AG29" s="27"/>
     </row>
-    <row r="30" ht="13.55" customHeight="1">
-      <c r="A30" t="s" s="21">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s" s="28">
+    <row r="30" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s" s="21">
-        <v>56</v>
-      </c>
-      <c r="D30" t="s" s="21">
-        <v>56</v>
+      <c r="C30" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -2991,18 +3067,18 @@
       <c r="AF30" s="26"/>
       <c r="AG30" s="27"/>
     </row>
-    <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" t="s" s="21">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s" s="28">
+    <row r="31" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C31" t="s" s="21">
-        <v>58</v>
-      </c>
-      <c r="D31" t="s" s="21">
-        <v>58</v>
+      <c r="C31" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>56</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -3034,18 +3110,18 @@
       <c r="AF31" s="26"/>
       <c r="AG31" s="27"/>
     </row>
-    <row r="32" ht="13.55" customHeight="1">
-      <c r="A32" t="s" s="21">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s" s="28">
+    <row r="32" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C32" t="s" s="21">
-        <v>60</v>
-      </c>
-      <c r="D32" t="s" s="21">
-        <v>60</v>
+      <c r="C32" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -3077,18 +3153,18 @@
       <c r="AF32" s="26"/>
       <c r="AG32" s="27"/>
     </row>
-    <row r="33" ht="13.55" customHeight="1">
-      <c r="A33" t="s" s="21">
-        <v>61</v>
-      </c>
-      <c r="B33" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C33" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D33" t="b" s="23">
-        <v>0</v>
+    <row r="33" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -3120,18 +3196,18 @@
       <c r="AF33" s="26"/>
       <c r="AG33" s="27"/>
     </row>
-    <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" t="s" s="21">
-        <v>62</v>
-      </c>
-      <c r="B34" t="s" s="22">
+    <row r="34" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C34" t="b" s="23">
-        <v>1</v>
-      </c>
-      <c r="D34" t="b" s="23">
-        <v>1</v>
+      <c r="C34" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="23" t="b">
+        <v>0</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
@@ -3163,11 +3239,19 @@
       <c r="AF34" s="26"/>
       <c r="AG34" s="27"/>
     </row>
-    <row r="35" ht="13.55" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="30"/>
+    <row r="35" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="23" t="b">
+        <v>1</v>
+      </c>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
@@ -3198,126 +3282,118 @@
       <c r="AF35" s="26"/>
       <c r="AG35" s="27"/>
     </row>
-    <row r="36" ht="13.55" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="17"/>
-      <c r="V36" s="17"/>
-      <c r="W36" s="17"/>
-      <c r="X36" s="17"/>
-      <c r="Y36" s="17"/>
-      <c r="Z36" s="17"/>
-      <c r="AA36" s="17"/>
-      <c r="AB36" s="17"/>
-      <c r="AC36" s="17"/>
-      <c r="AD36" s="17"/>
-      <c r="AE36" s="17"/>
-      <c r="AF36" s="17"/>
-      <c r="AG36" s="17"/>
-    </row>
-    <row r="37" ht="18.75" customHeight="1">
-      <c r="A37" t="s" s="19">
+    <row r="36" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="26"/>
+      <c r="X36" s="26"/>
+      <c r="Y36" s="26"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="26"/>
+      <c r="AC36" s="26"/>
+      <c r="AD36" s="26"/>
+      <c r="AE36" s="26"/>
+      <c r="AF36" s="26"/>
+      <c r="AG36" s="27"/>
+    </row>
+    <row r="37" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="17"/>
+      <c r="AB37" s="17"/>
+      <c r="AC37" s="17"/>
+      <c r="AD37" s="17"/>
+      <c r="AE37" s="17"/>
+      <c r="AF37" s="17"/>
+      <c r="AG37" s="17"/>
+    </row>
+    <row r="38" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
-      <c r="AD37" s="20"/>
-      <c r="AE37" s="20"/>
-      <c r="AF37" s="20"/>
-      <c r="AG37" s="20"/>
-    </row>
-    <row r="38" ht="13.55" customHeight="1">
-      <c r="A38" t="s" s="21">
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="20"/>
+      <c r="AG38" s="20"/>
+    </row>
+    <row r="39" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B38" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="C38" s="23">
-        <v>5</v>
-      </c>
-      <c r="D38" s="23">
-        <v>5</v>
-      </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="T38" s="25"/>
-      <c r="U38" s="26"/>
-      <c r="V38" s="26"/>
-      <c r="W38" s="26"/>
-      <c r="X38" s="26"/>
-      <c r="Y38" s="26"/>
-      <c r="Z38" s="26"/>
-      <c r="AA38" s="26"/>
-      <c r="AB38" s="26"/>
-      <c r="AC38" s="26"/>
-      <c r="AD38" s="26"/>
-      <c r="AE38" s="26"/>
-      <c r="AF38" s="26"/>
-      <c r="AG38" s="27"/>
-    </row>
-    <row r="39" ht="13.55" customHeight="1">
-      <c r="A39" t="s" s="21">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s" s="22">
+      <c r="B39" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="23">
@@ -3356,18 +3432,18 @@
       <c r="AF39" s="26"/>
       <c r="AG39" s="27"/>
     </row>
-    <row r="40" ht="13.55" customHeight="1">
-      <c r="A40" t="s" s="21">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s" s="22">
+    <row r="40" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D40" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -3399,18 +3475,18 @@
       <c r="AF40" s="26"/>
       <c r="AG40" s="27"/>
     </row>
-    <row r="41" ht="13.55" customHeight="1">
-      <c r="A41" t="s" s="21">
-        <v>68</v>
-      </c>
-      <c r="B41" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C41" t="b" s="23">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s" s="21">
-        <v>69</v>
+    <row r="41" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="23">
+        <v>1</v>
+      </c>
+      <c r="D41" s="23">
+        <v>1</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -3442,18 +3518,18 @@
       <c r="AF41" s="26"/>
       <c r="AG41" s="27"/>
     </row>
-    <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="B42" t="s" s="28">
-        <v>65</v>
-      </c>
-      <c r="C42" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="D42" s="23">
-        <v>0.75</v>
+    <row r="42" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3485,18 +3561,18 @@
       <c r="AF42" s="26"/>
       <c r="AG42" s="27"/>
     </row>
-    <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" t="s" s="21">
-        <v>71</v>
-      </c>
-      <c r="B43" t="s" s="22">
-        <v>17</v>
-      </c>
-      <c r="C43" t="b" s="23">
-        <v>1</v>
-      </c>
-      <c r="D43" t="b" s="23">
-        <v>1</v>
+    <row r="43" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="D43" s="23">
+        <v>0.75</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -3528,18 +3604,18 @@
       <c r="AF43" s="26"/>
       <c r="AG43" s="27"/>
     </row>
-    <row r="44" ht="13.55" customHeight="1">
-      <c r="A44" t="s" s="21">
-        <v>72</v>
-      </c>
-      <c r="B44" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="C44" s="23">
-        <v>-0.5</v>
-      </c>
-      <c r="D44" s="23">
-        <v>-0.5</v>
+    <row r="44" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="23" t="b">
+        <v>1</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -3571,18 +3647,18 @@
       <c r="AF44" s="26"/>
       <c r="AG44" s="27"/>
     </row>
-    <row r="45" ht="13.55" customHeight="1">
-      <c r="A45" t="s" s="21">
-        <v>73</v>
-      </c>
-      <c r="B45" t="s" s="22">
+    <row r="45" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="D45" s="23">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -3614,18 +3690,18 @@
       <c r="AF45" s="26"/>
       <c r="AG45" s="27"/>
     </row>
-    <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" t="s" s="21">
-        <v>74</v>
-      </c>
-      <c r="B46" t="s" s="22">
+    <row r="46" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="D46" s="23">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
@@ -3657,11 +3733,19 @@
       <c r="AF46" s="26"/>
       <c r="AG46" s="27"/>
     </row>
-    <row r="47" ht="13.55" customHeight="1">
-      <c r="A47" s="24"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
+    <row r="47" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="23">
+        <v>1.05</v>
+      </c>
+      <c r="D47" s="23">
+        <v>1.05</v>
+      </c>
       <c r="E47" s="24"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
@@ -3692,133 +3776,125 @@
       <c r="AF47" s="26"/>
       <c r="AG47" s="27"/>
     </row>
-    <row r="48" ht="13.55" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="17"/>
-      <c r="U48" s="17"/>
-      <c r="V48" s="17"/>
-      <c r="W48" s="17"/>
-      <c r="X48" s="17"/>
-      <c r="Y48" s="17"/>
-      <c r="Z48" s="17"/>
-      <c r="AA48" s="17"/>
-      <c r="AB48" s="17"/>
-      <c r="AC48" s="17"/>
-      <c r="AD48" s="17"/>
-      <c r="AE48" s="17"/>
-      <c r="AF48" s="17"/>
-      <c r="AG48" s="17"/>
-    </row>
-    <row r="49" ht="18.75" customHeight="1">
-      <c r="A49" t="s" s="19">
+    <row r="48" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="24"/>
+      <c r="Q48" s="24"/>
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="25"/>
+      <c r="U48" s="26"/>
+      <c r="V48" s="26"/>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
+      <c r="Y48" s="26"/>
+      <c r="Z48" s="26"/>
+      <c r="AA48" s="26"/>
+      <c r="AB48" s="26"/>
+      <c r="AC48" s="26"/>
+      <c r="AD48" s="26"/>
+      <c r="AE48" s="26"/>
+      <c r="AF48" s="26"/>
+      <c r="AG48" s="27"/>
+    </row>
+    <row r="49" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="17"/>
+      <c r="Z49" s="17"/>
+      <c r="AA49" s="17"/>
+      <c r="AB49" s="17"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+      <c r="AE49" s="17"/>
+      <c r="AF49" s="17"/>
+      <c r="AG49" s="17"/>
+    </row>
+    <row r="50" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="20"/>
-      <c r="U49" s="20"/>
-      <c r="V49" s="20"/>
-      <c r="W49" s="20"/>
-      <c r="X49" s="20"/>
-      <c r="Y49" s="20"/>
-      <c r="Z49" s="20"/>
-      <c r="AA49" s="20"/>
-      <c r="AB49" s="20"/>
-      <c r="AC49" s="20"/>
-      <c r="AD49" s="20"/>
-      <c r="AE49" s="20"/>
-      <c r="AF49" s="20"/>
-      <c r="AG49" s="20"/>
-    </row>
-    <row r="50" ht="13.55" customHeight="1">
-      <c r="A50" t="s" s="21">
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
+      <c r="Z50" s="20"/>
+      <c r="AA50" s="20"/>
+      <c r="AB50" s="20"/>
+      <c r="AC50" s="20"/>
+      <c r="AD50" s="20"/>
+      <c r="AE50" s="20"/>
+      <c r="AF50" s="20"/>
+      <c r="AG50" s="20"/>
+    </row>
+    <row r="51" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B50" t="s" s="22">
+      <c r="B51" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C50" t="s" s="21">
+      <c r="C51" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D50" t="s" s="21">
+      <c r="D51" s="21" t="s">
         <v>77</v>
-      </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="25"/>
-      <c r="U50" s="26"/>
-      <c r="V50" s="26"/>
-      <c r="W50" s="26"/>
-      <c r="X50" s="26"/>
-      <c r="Y50" s="26"/>
-      <c r="Z50" s="26"/>
-      <c r="AA50" s="26"/>
-      <c r="AB50" s="26"/>
-      <c r="AC50" s="26"/>
-      <c r="AD50" s="26"/>
-      <c r="AE50" s="26"/>
-      <c r="AF50" s="26"/>
-      <c r="AG50" s="27"/>
-    </row>
-    <row r="51" ht="13.55" customHeight="1">
-      <c r="A51" t="s" s="21">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s" s="22">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s" s="21">
-        <v>79</v>
-      </c>
-      <c r="D51" t="s" s="21">
-        <v>79</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
@@ -3850,18 +3926,18 @@
       <c r="AF51" s="26"/>
       <c r="AG51" s="27"/>
     </row>
-    <row r="52" ht="13.55" customHeight="1">
-      <c r="A52" t="s" s="21">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s" s="22">
+    <row r="52" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C52" t="s" s="21">
-        <v>81</v>
-      </c>
-      <c r="D52" t="s" s="21">
-        <v>81</v>
+      <c r="C52" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="E52" s="24"/>
       <c r="F52" s="24"/>
@@ -3893,18 +3969,18 @@
       <c r="AF52" s="26"/>
       <c r="AG52" s="27"/>
     </row>
-    <row r="53" ht="13.55" customHeight="1">
-      <c r="A53" t="s" s="21">
-        <v>82</v>
-      </c>
-      <c r="B53" t="s" s="22">
+    <row r="53" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C53" t="s" s="21">
-        <v>83</v>
-      </c>
-      <c r="D53" t="s" s="21">
-        <v>83</v>
+      <c r="C53" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -3936,18 +4012,18 @@
       <c r="AF53" s="26"/>
       <c r="AG53" s="27"/>
     </row>
-    <row r="54" ht="13.55" customHeight="1">
-      <c r="A54" t="s" s="21">
-        <v>84</v>
-      </c>
-      <c r="B54" t="s" s="22">
+    <row r="54" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C54" t="s" s="21">
-        <v>85</v>
-      </c>
-      <c r="D54" t="s" s="21">
-        <v>85</v>
+      <c r="C54" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -3979,18 +4055,18 @@
       <c r="AF54" s="26"/>
       <c r="AG54" s="27"/>
     </row>
-    <row r="55" ht="13.55" customHeight="1">
-      <c r="A55" t="s" s="21">
-        <v>86</v>
-      </c>
-      <c r="B55" t="s" s="22">
+    <row r="55" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C55" t="s" s="21">
-        <v>87</v>
-      </c>
-      <c r="D55" t="s" s="21">
-        <v>87</v>
+      <c r="C55" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -4022,18 +4098,18 @@
       <c r="AF55" s="26"/>
       <c r="AG55" s="27"/>
     </row>
-    <row r="56" ht="13.55" customHeight="1">
-      <c r="A56" t="s" s="21">
-        <v>88</v>
-      </c>
-      <c r="B56" t="s" s="22">
+    <row r="56" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C56" t="s" s="21">
-        <v>89</v>
-      </c>
-      <c r="D56" t="s" s="21">
-        <v>89</v>
+      <c r="C56" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>87</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
@@ -4065,18 +4141,18 @@
       <c r="AF56" s="26"/>
       <c r="AG56" s="27"/>
     </row>
-    <row r="57" ht="13.55" customHeight="1">
-      <c r="A57" t="s" s="21">
-        <v>90</v>
-      </c>
-      <c r="B57" t="s" s="22">
+    <row r="57" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C57" t="s" s="21">
-        <v>91</v>
-      </c>
-      <c r="D57" t="s" s="21">
-        <v>91</v>
+      <c r="C57" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
@@ -4108,18 +4184,18 @@
       <c r="AF57" s="26"/>
       <c r="AG57" s="27"/>
     </row>
-    <row r="58" ht="13.55" customHeight="1">
-      <c r="A58" t="s" s="21">
-        <v>92</v>
-      </c>
-      <c r="B58" t="s" s="22">
+    <row r="58" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C58" t="s" s="21">
-        <v>93</v>
-      </c>
-      <c r="D58" t="s" s="21">
-        <v>93</v>
+      <c r="C58" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
@@ -4151,9 +4227,52 @@
       <c r="AF58" s="26"/>
       <c r="AG58" s="27"/>
     </row>
+    <row r="59" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="24"/>
+      <c r="K59" s="24"/>
+      <c r="L59" s="24"/>
+      <c r="M59" s="24"/>
+      <c r="N59" s="24"/>
+      <c r="O59" s="24"/>
+      <c r="P59" s="24"/>
+      <c r="Q59" s="24"/>
+      <c r="R59" s="24"/>
+      <c r="S59" s="24"/>
+      <c r="T59" s="25"/>
+      <c r="U59" s="26"/>
+      <c r="V59" s="26"/>
+      <c r="W59" s="26"/>
+      <c r="X59" s="26"/>
+      <c r="Y59" s="26"/>
+      <c r="Z59" s="26"/>
+      <c r="AA59" s="26"/>
+      <c r="AB59" s="26"/>
+      <c r="AC59" s="26"/>
+      <c r="AD59" s="26"/>
+      <c r="AE59" s="26"/>
+      <c r="AF59" s="26"/>
+      <c r="AG59" s="27"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
More updates to allow for simulated_vehicles.csv instead of cost_clouds.csv. Rolled back to_numeric conversions in producer.py, and flagged simulated_vehicles_id field as non-numeric.
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBolon\PycharmProjects\EPA_OMEGA_Model\usepa_omega2\test_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23A305A-EDC7-4BA8-8C29-1B5E7901C31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31BA482-AEA6-4B33-A4CD-5A9DB814D168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1095" windowWidth="17895" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17925" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="1" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>Cost File</t>
   </si>
   <si>
-    <t>cost_clouds.csv</t>
-  </si>
-  <si>
     <t>GHG Standards File</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>ghg_credits.csv</t>
+  </si>
+  <si>
+    <t>simulated_vehicles.csv</t>
   </si>
 </sst>
 </file>
@@ -1808,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2817,10 +2817,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="26" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>48</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
@@ -2897,16 +2897,16 @@
     </row>
     <row r="27" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
@@ -2940,16 +2940,16 @@
     </row>
     <row r="28" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -2983,16 +2983,16 @@
     </row>
     <row r="29" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -3026,16 +3026,16 @@
     </row>
     <row r="30" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="31" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -3112,16 +3112,16 @@
     </row>
     <row r="32" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -3155,16 +3155,16 @@
     </row>
     <row r="33" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="34" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>17</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="35" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>17</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="38" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -3391,10 +3391,10 @@
     </row>
     <row r="39" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="C39" s="23">
         <v>5</v>
@@ -3434,10 +3434,10 @@
     </row>
     <row r="40" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="23">
         <v>5</v>
@@ -3477,10 +3477,10 @@
     </row>
     <row r="41" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="23">
         <v>1</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="42" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>17</v>
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -3563,10 +3563,10 @@
     </row>
     <row r="43" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="23">
         <v>0.75</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="44" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>17</v>
@@ -3649,10 +3649,10 @@
     </row>
     <row r="45" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="23">
         <v>-0.5</v>
@@ -3692,10 +3692,10 @@
     </row>
     <row r="46" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="23">
         <v>0.95</v>
@@ -3735,10 +3735,10 @@
     </row>
     <row r="47" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="23">
         <v>1.05</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="50" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -3885,16 +3885,16 @@
     </row>
     <row r="51" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="52" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E52" s="24"/>
       <c r="F52" s="24"/>
@@ -3971,16 +3971,16 @@
     </row>
     <row r="53" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -4014,16 +4014,16 @@
     </row>
     <row r="54" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -4057,16 +4057,16 @@
     </row>
     <row r="55" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -4100,16 +4100,16 @@
     </row>
     <row r="56" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B56" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
@@ -4143,16 +4143,16 @@
     </row>
     <row r="57" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
@@ -4186,16 +4186,16 @@
     </row>
     <row r="58" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
@@ -4229,16 +4229,16 @@
     </row>
     <row r="59" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>

</xml_diff>

<commit_message>
added sales incentives (e.g. BEV multipliers) fixed an issue with composite vehicle target CO2 Mg and source vehicle target Mg not matching up after decomposition and thereby causing a discrepancy between the credit history and actual cert performance
</commit_message>
<xml_diff>
--- a/usepa_omega2/test_inputs/multiple_session_batch.xlsx
+++ b/usepa_omega2/test_inputs/multiple_session_batch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
   <si>
     <t>multiple_session_batch</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ghg_standards-flat.csv</t>
+  </si>
+  <si>
+    <t>GHG Standards Sales Incentives File</t>
+  </si>
+  <si>
+    <t>ghg_standards-sales_incentives.csv</t>
   </si>
   <si>
     <t>GHG Standards Fuels File</t>
@@ -314,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -326,13 +332,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,18 +352,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -361,32 +378,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
+      <left>
+        <color indexed="9"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
+      <right>
+        <color indexed="9"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
+      <top>
+        <color indexed="9"/>
       </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+      <bottom>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -394,74 +396,98 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,50 +497,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -534,8 +557,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -554,10 +580,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -734,11 +760,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -747,34 +776,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1022,12 +1051,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1318,7 +1347,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1599,761 +1628,743 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D59"/>
+  <dimension ref="A1:ALL60"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" defaultGridColor="0" colorId="9"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="36.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6719" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6719" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.3516" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.6719" style="2" customWidth="1"/>
+    <col min="5" max="1000" width="8.35156" style="2" customWidth="1"/>
+    <col min="1001" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" s="3" customFormat="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="4">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+    </row>
+    <row r="4" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="10">
+      <c r="B4" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+    </row>
+    <row r="5" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="B5" t="s" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s" s="10">
+      <c r="B6" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
+    </row>
+    <row r="7" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s" s="10">
+      <c r="B7" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s" s="11">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="8">
+    </row>
+    <row r="8" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="9">
         <v>12</v>
       </c>
-      <c r="B8" t="s" s="9">
+      <c r="B8" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" t="s" s="11">
         <v>14</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
+    </row>
+    <row r="9" s="3" customFormat="1" ht="20.05" customHeight="1">
       <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
+    </row>
+    <row r="10" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
+    </row>
+    <row r="11" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B11" t="s" s="9">
+      <c r="B11" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C11" t="b" s="14">
+      <c r="C11" t="b" s="13">
         <v>1</v>
       </c>
-      <c r="D11" t="b" s="14">
+      <c r="D11" t="b" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
+    <row r="12" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="9">
         <v>18</v>
       </c>
-      <c r="B12" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s" s="10">
+      <c r="B12" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s" s="11">
         <v>19</v>
       </c>
-      <c r="D12" t="s" s="10">
+      <c r="D12" t="s" s="11">
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
+    <row r="13" s="3" customFormat="1" ht="20.05" customHeight="1">
       <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="8">
+    </row>
+    <row r="14" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="8">
+    </row>
+    <row r="15" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="9">
         <v>22</v>
       </c>
-      <c r="B15" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s" s="10">
+      <c r="B15" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s" s="11">
         <v>23</v>
       </c>
-      <c r="D15" t="s" s="10">
+      <c r="D15" t="s" s="11">
         <v>23</v>
       </c>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="8">
+    <row r="16" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="9">
         <v>24</v>
       </c>
-      <c r="B16" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s" s="10">
+      <c r="B16" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s" s="11">
         <v>25</v>
       </c>
-      <c r="D16" t="s" s="10">
+      <c r="D16" t="s" s="11">
         <v>25</v>
       </c>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="8">
+    <row r="17" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A17" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="B17" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s" s="10">
+      <c r="B17" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="D17" t="s" s="10">
+      <c r="D17" t="s" s="11">
         <v>27</v>
       </c>
     </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="8">
+    <row r="18" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A18" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B18" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s" s="10">
+      <c r="B18" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s" s="11">
         <v>29</v>
       </c>
-      <c r="D18" t="s" s="10">
+      <c r="D18" t="s" s="11">
         <v>29</v>
       </c>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="8">
+    <row r="19" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B19" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s" s="10">
+      <c r="B19" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s" s="11">
         <v>31</v>
       </c>
-      <c r="D19" t="s" s="10">
+      <c r="D19" t="s" s="11">
         <v>31</v>
       </c>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="8">
+    <row r="20" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="9">
         <v>32</v>
       </c>
-      <c r="B20" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s" s="10">
+      <c r="B20" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s" s="11">
         <v>33</v>
       </c>
-      <c r="D20" t="s" s="10">
+      <c r="D20" t="s" s="11">
         <v>33</v>
       </c>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="8">
+    <row r="21" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="9">
         <v>34</v>
       </c>
-      <c r="B21" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s" s="10">
+      <c r="B21" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s" s="11">
         <v>35</v>
       </c>
-      <c r="D21" t="s" s="10">
+      <c r="D21" t="s" s="11">
         <v>35</v>
       </c>
     </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="8">
+    <row r="22" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B22" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s" s="10">
+      <c r="B22" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s" s="11">
         <v>37</v>
       </c>
-      <c r="D22" t="s" s="10">
+      <c r="D22" t="s" s="11">
         <v>37</v>
       </c>
     </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="8">
+    <row r="23" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="B23" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s" s="10">
+      <c r="B23" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s" s="11">
         <v>39</v>
       </c>
-      <c r="D23" t="s" s="10">
+      <c r="D23" t="s" s="11">
         <v>39</v>
       </c>
     </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="8">
+    <row r="24" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="9">
         <v>40</v>
       </c>
-      <c r="B24" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s" s="10">
+      <c r="B24" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s" s="11">
         <v>41</v>
       </c>
-      <c r="D24" t="s" s="10">
+      <c r="D24" t="s" s="11">
         <v>41</v>
       </c>
     </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="8">
+    <row r="25" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A25" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="B25" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s" s="10">
+      <c r="B25" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s" s="11">
         <v>43</v>
       </c>
-      <c r="D25" t="s" s="10">
+      <c r="D25" t="s" s="11">
         <v>43</v>
       </c>
     </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="8">
+    <row r="26" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A26" t="s" s="9">
         <v>44</v>
       </c>
-      <c r="B26" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s" s="10">
+      <c r="B26" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s" s="11">
         <v>45</v>
       </c>
-      <c r="D26" t="s" s="10">
+      <c r="D26" t="s" s="11">
         <v>45</v>
       </c>
     </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="8">
+    <row r="27" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A27" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="B27" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s" s="10">
+      <c r="B27" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s" s="11">
         <v>47</v>
       </c>
-      <c r="D27" t="s" s="10">
+      <c r="D27" t="s" s="11">
         <v>47</v>
       </c>
     </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="8">
+    <row r="28" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A28" t="s" s="9">
         <v>48</v>
       </c>
-      <c r="B28" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s" s="10">
+      <c r="B28" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s" s="11">
         <v>49</v>
       </c>
-      <c r="D28" t="s" s="10">
+      <c r="D28" t="s" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="8">
+    <row r="29" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A29" t="s" s="9">
         <v>51</v>
       </c>
-      <c r="B29" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s" s="10">
+      <c r="B29" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s" s="11">
         <v>52</v>
       </c>
-      <c r="D29" t="s" s="10">
+      <c r="D29" t="s" s="11">
         <v>52</v>
       </c>
     </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="8">
+    <row r="30" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="9">
         <v>53</v>
       </c>
-      <c r="B30" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s" s="10">
+      <c r="B30" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s" s="11">
         <v>54</v>
       </c>
-      <c r="D30" t="s" s="10">
+      <c r="D30" t="s" s="11">
         <v>54</v>
       </c>
     </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="8">
+    <row r="31" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B31" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s" s="10">
+      <c r="B31" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s" s="11">
         <v>56</v>
       </c>
-      <c r="D31" t="s" s="10">
+      <c r="D31" t="s" s="11">
         <v>56</v>
       </c>
     </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="8">
+    <row r="32" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A32" t="s" s="9">
         <v>57</v>
       </c>
-      <c r="B32" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s" s="10">
+      <c r="B32" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s" s="11">
         <v>58</v>
       </c>
-      <c r="D32" t="s" s="10">
+      <c r="D32" t="s" s="11">
         <v>58</v>
       </c>
     </row>
-    <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="8">
+    <row r="33" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A33" t="s" s="9">
         <v>59</v>
       </c>
-      <c r="B33" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s" s="10">
+      <c r="B33" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s" s="11">
         <v>60</v>
       </c>
-      <c r="D33" t="s" s="10">
+      <c r="D33" t="s" s="11">
         <v>60</v>
       </c>
     </row>
-    <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" t="s" s="8">
+    <row r="34" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="9">
         <v>61</v>
       </c>
-      <c r="B34" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s" s="10">
+      <c r="B34" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s" s="11">
         <v>62</v>
       </c>
-      <c r="D34" t="s" s="10">
+      <c r="D34" t="s" s="11">
         <v>62</v>
       </c>
     </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" t="s" s="8">
+    <row r="35" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A35" t="s" s="9">
         <v>63</v>
       </c>
-      <c r="B35" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s" s="10">
+      <c r="B35" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s" s="11">
         <v>64</v>
       </c>
-      <c r="D35" t="s" s="10">
+      <c r="D35" t="s" s="11">
         <v>64</v>
       </c>
     </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" t="s" s="8">
+    <row r="36" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="9">
         <v>65</v>
       </c>
-      <c r="B36" t="s" s="9">
+      <c r="B36" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s" s="11">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s" s="11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A37" t="s" s="9">
+        <v>67</v>
+      </c>
+      <c r="B37" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C36" t="b" s="14">
+      <c r="C37" t="b" s="13">
         <v>0</v>
       </c>
-      <c r="D36" t="b" s="14">
+      <c r="D37" t="b" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="B37" t="s" s="9">
+    <row r="38" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A38" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C37" t="b" s="14">
+      <c r="C38" t="b" s="13">
         <v>1</v>
       </c>
-      <c r="D37" t="b" s="14">
+      <c r="D38" t="b" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="8">
-        <v>67</v>
-      </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s" s="9">
+    <row r="39" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A39" s="12"/>
+    </row>
+    <row r="40" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A40" t="s" s="9">
         <v>69</v>
       </c>
-      <c r="C40" s="14">
+    </row>
+    <row r="41" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A41" t="s" s="9">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C41" s="13">
         <v>5</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D41" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" t="s" s="8">
-        <v>70</v>
-      </c>
-      <c r="B41" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C41" s="14">
+    <row r="42" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A42" t="s" s="9">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C42" s="13">
         <v>5</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D42" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" t="s" s="8">
+    <row r="43" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A43" t="s" s="9">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s" s="10">
         <v>71</v>
       </c>
-      <c r="B42" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C42" s="14">
+      <c r="C43" s="13">
         <v>1</v>
       </c>
-      <c r="D42" s="14">
+      <c r="D43" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="B43" t="s" s="9">
+    <row r="44" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A44" t="s" s="9">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C43" t="b" s="14">
+      <c r="C44" t="b" s="13">
         <v>0</v>
       </c>
-      <c r="D43" t="s" s="10">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" t="s" s="8">
-        <v>74</v>
-      </c>
-      <c r="B44" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C44" s="14">
+      <c r="D44" t="s" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A45" t="s" s="9">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C45" s="13">
         <v>0.75</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D45" s="13">
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="8">
-        <v>75</v>
-      </c>
-      <c r="B45" t="s" s="9">
+    <row r="46" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A46" t="s" s="9">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C45" t="b" s="14">
+      <c r="C46" t="b" s="13">
         <v>1</v>
       </c>
-      <c r="D45" t="b" s="14">
+      <c r="D46" t="b" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="8">
-        <v>76</v>
-      </c>
-      <c r="B46" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C46" s="14">
+    <row r="47" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A47" t="s" s="9">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C47" s="13">
         <v>-0.5</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D47" s="13">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="8">
-        <v>77</v>
-      </c>
-      <c r="B47" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C47" s="14">
+    <row r="48" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A48" t="s" s="9">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C48" s="13">
         <v>0.95</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D48" s="13">
         <v>0.95</v>
       </c>
     </row>
-    <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="8">
-        <v>78</v>
-      </c>
-      <c r="B48" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="C48" s="14">
+    <row r="49" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A49" t="s" s="9">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="C49" s="13">
         <v>1.05</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D49" s="13">
         <v>1.05</v>
       </c>
     </row>
-    <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="12"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="8">
-        <v>79</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="8">
-        <v>80</v>
-      </c>
-      <c r="B51" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C51" t="s" s="10">
+    <row r="50" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A50" s="12"/>
+    </row>
+    <row r="51" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A51" t="s" s="9">
         <v>81</v>
       </c>
-      <c r="D51" t="s" s="10">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" t="s" s="8">
+    </row>
+    <row r="52" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A52" t="s" s="9">
         <v>82</v>
       </c>
-      <c r="B52" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C52" t="s" s="10">
+      <c r="B52" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="D52" t="s" s="10">
+      <c r="D52" t="s" s="11">
         <v>83</v>
       </c>
     </row>
-    <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" t="s" s="8">
+    <row r="53" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A53" t="s" s="9">
         <v>84</v>
       </c>
-      <c r="B53" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s" s="10">
+      <c r="B53" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="D53" t="s" s="10">
+      <c r="D53" t="s" s="11">
         <v>85</v>
       </c>
     </row>
-    <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="8">
+    <row r="54" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A54" t="s" s="9">
         <v>86</v>
       </c>
-      <c r="B54" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C54" t="s" s="10">
+      <c r="B54" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s" s="11">
         <v>87</v>
       </c>
-      <c r="D54" t="s" s="10">
+      <c r="D54" t="s" s="11">
         <v>87</v>
       </c>
     </row>
-    <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" t="s" s="8">
+    <row r="55" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A55" t="s" s="9">
         <v>88</v>
       </c>
-      <c r="B55" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C55" t="s" s="10">
+      <c r="B55" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s" s="11">
         <v>89</v>
       </c>
-      <c r="D55" t="s" s="10">
+      <c r="D55" t="s" s="11">
         <v>89</v>
       </c>
     </row>
-    <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" t="s" s="8">
+    <row r="56" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A56" t="s" s="9">
         <v>90</v>
       </c>
-      <c r="B56" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C56" t="s" s="10">
+      <c r="B56" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s" s="11">
         <v>91</v>
       </c>
-      <c r="D56" t="s" s="10">
+      <c r="D56" t="s" s="11">
         <v>91</v>
       </c>
     </row>
-    <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" t="s" s="8">
+    <row r="57" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A57" t="s" s="9">
         <v>92</v>
       </c>
-      <c r="B57" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C57" t="s" s="10">
+      <c r="B57" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s" s="11">
         <v>93</v>
       </c>
-      <c r="D57" t="s" s="10">
+      <c r="D57" t="s" s="11">
         <v>93</v>
       </c>
     </row>
-    <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" t="s" s="8">
+    <row r="58" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A58" t="s" s="9">
         <v>94</v>
       </c>
-      <c r="B58" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C58" t="s" s="10">
+      <c r="B58" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="D58" t="s" s="10">
+      <c r="D58" t="s" s="11">
         <v>95</v>
       </c>
     </row>
-    <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" t="s" s="8">
+    <row r="59" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A59" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="B59" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="C59" t="s" s="10">
+      <c r="B59" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s" s="11">
         <v>97</v>
       </c>
-      <c r="D59" t="s" s="10">
+      <c r="D59" t="s" s="11">
         <v>97</v>
+      </c>
+    </row>
+    <row r="60" s="3" customFormat="1" ht="20.05" customHeight="1">
+      <c r="A60" t="s" s="9">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s" s="11">
+        <v>99</v>
+      </c>
+      <c r="D60" t="s" s="11">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>